<commit_message>
Entry Screens and Password Change Screen yet to be done.
</commit_message>
<xml_diff>
--- a/Design/Normalisation.xlsx
+++ b/Design/Normalisation.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Imran Rahman\Documents\Year 13\Computing\git\COMP4Coursework\Design\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -966,7 +971,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -976,7 +981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>

</xml_diff>